<commit_message>
update figure for 2020/12 draft
</commit_message>
<xml_diff>
--- a/Analysis/figTbl_guidebook/tbl_tradeOff&decomposition_FR100.xlsx
+++ b/Analysis/figTbl_guidebook/tbl_tradeOff&decomposition_FR100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim_riskSharing\Analysis\figTbl_guidebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91292F3C-0903-4512-9DB7-9C84A6900FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55D58E6-90EB-479E-A679-05D89BDB4A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="126">
   <si>
     <t>runname</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>PV of salary</t>
+  </si>
+  <si>
+    <t>Imact on PV ERC, plan starting with 100% funded ratio</t>
   </si>
 </sst>
 </file>
@@ -4449,7 +4452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AC6BED-6E6B-43AC-B690-CD2222CF03DF}">
   <dimension ref="A1:XFA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:E24"/>
     </sheetView>
   </sheetViews>
@@ -22260,10 +22263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00DE40E-A194-4591-BD3E-86222361CF3A}">
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B1" sqref="B1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22272,130 +22275,141 @@
     <col min="3" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>79</v>
-      </c>
+    <row r="1" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="78" t="s">
+      <c r="C2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="74">
+      <c r="C3" s="74">
         <v>-2.1031268331070836E-2</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D3" s="74">
         <v>0</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E3" s="74">
         <v>-2.1031268331070836E-2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="78" t="s">
+    <row r="4" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="74">
+      <c r="C4" s="74">
         <v>-7.9358240020854703E-2</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D4" s="74">
         <v>7.1278756261980644E-3</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E4" s="74">
         <v>-8.6486115647052775E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+    <row r="5" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="74">
+      <c r="C5" s="74">
         <v>-4.4601642915159882E-2</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D5" s="74">
         <v>-1.9826737672217279E-16</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E5" s="74">
         <v>-4.4601642915159681E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="78" t="s">
+    <row r="6" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="74">
+      <c r="C6" s="74">
         <v>-9.7585429625515946E-2</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D6" s="74">
         <v>1.3217825114811519E-16</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E6" s="74">
         <v>-9.7585429625516085E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="78" t="s">
+    <row r="7" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="74">
+      <c r="C7" s="74">
         <v>-0.29806491883568892</v>
-      </c>
-      <c r="D6" s="74">
-        <v>-2.6272326951113999E-2</v>
-      </c>
-      <c r="E6" s="74">
-        <v>-0.27179259188457494</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="74">
-        <v>-0.30592627284373358</v>
       </c>
       <c r="D7" s="74">
         <v>-2.6272326951113999E-2</v>
       </c>
       <c r="E7" s="74">
+        <v>-0.27179259188457494</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="74">
+        <v>-0.30592627284373358</v>
+      </c>
+      <c r="D8" s="74">
+        <v>-2.6272326951113999E-2</v>
+      </c>
+      <c r="E8" s="74">
         <v>-0.2796539458926196</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="78" t="s">
+    <row r="9" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C9" s="74">
         <v>-0.28263742558498173</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D9" s="74">
         <v>-2.9834796923620629E-3</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E9" s="74">
         <v>-0.27965394589261966</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="80" t="s">
+    <row r="10" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C10" s="81">
         <v>-0.10597687312299794</v>
       </c>
-      <c r="D9" s="81">
+      <c r="D10" s="81">
         <v>9.5349502490609112E-2</v>
       </c>
-      <c r="E9" s="81">
+      <c r="E10" s="81">
         <v>-0.20132637561360706</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>